<commit_message>
atualização maio. comenta linhas do código para evitar confusão.
</commit_message>
<xml_diff>
--- a/base-siafi/dados/tg_ Base Siafi 2020 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
+++ b/base-siafi/dados/tg_ Base Siafi 2020 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="67">
   <si>
     <t>tg_ Base Siafi 2020 so RGPS Pgtos Totais Esf-Acao-Mod</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Filtro do relatório:</t>
   </si>
   <si>
-    <t>({Item Informação} = 56:PAGAMENTOS TOTAIS (EXERCICIO E RAP)) E ({Órgão UGE - Orçam. Fiscal S/N} = PERTENCE) E ({Unidade Orçamentária} = 40904:FUNDO DO REGIME GERAL DA PREVID.SOCIAL- FRGPS, 55902:FUNDO DO REGIME GERAL DA PREVID.SOCIAL-FRGPS, 33904:FUNDO DO REGIME GERAL DA PREVIDENCIA SOCIAL, 25917:FUNDO DO REGIME GERAL DE PREVIDENCIA SOCIAL) E ({Ano Lançamento} ({Número Ano}) = 2020)</t>
+    <t>({Item Informação} = 56:PAGAMENTOS TOTAIS (EXERCICIO E RAP)) E ({Órgão UGE - Orçam. Fiscal S/N} = PERTENCE) E ({Unidade Orçamentária} = 40904:FUNDO DO REGIME GERAL DA PREVID.SOCIAL- FRGPS, 55902:FUNDO DO REGIME GERAL DA PREVID.SOCIAL-FRGPS, 33904:FUNDO DO REGIME GERAL DA PREVIDENCIA SOCIAL, 25917:FUNDO DO REGIME GERAL DE PREVIDENCIA SOCIAL) E ({Ano Lançamento} ({Número Ano}) = 2020) E ({Mês Lançamento} ({Número Mês}) Entre 1 E 5)</t>
   </si>
   <si>
     <t>Páginas:</t>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAI/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">0625</t>
@@ -257,7 +263,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -684,43 +690,43 @@
         <v>34</v>
       </c>
       <c r="I15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" t="s">
         <v>50</v>
       </c>
-      <c r="J15" t="s">
+      <c r="S15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15" t="s">
         <v>51</v>
       </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" t="s">
-        <v>41</v>
-      </c>
-      <c r="P15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>43</v>
-      </c>
-      <c r="R15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S15" t="s">
-        <v>45</v>
-      </c>
-      <c r="T15" t="s">
-        <v>41</v>
-      </c>
       <c r="U15" s="1">
-        <v>759268717.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -749,10 +755,10 @@
         <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
         <v>37</v>
@@ -776,16 +782,16 @@
         <v>43</v>
       </c>
       <c r="R16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S16" t="s">
         <v>45</v>
       </c>
       <c r="T16" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="U16" s="1">
-        <v>636669876.37</v>
+        <v>759268717.55</v>
       </c>
     </row>
     <row r="17">
@@ -814,10 +820,10 @@
         <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
         <v>37</v>
@@ -841,16 +847,16 @@
         <v>43</v>
       </c>
       <c r="R17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S17" t="s">
         <v>45</v>
       </c>
       <c r="T17" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U17" s="1">
-        <v>797851921.26</v>
+        <v>636669876.37</v>
       </c>
     </row>
     <row r="18">
@@ -879,10 +885,10 @@
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
         <v>37</v>
@@ -906,16 +912,16 @@
         <v>43</v>
       </c>
       <c r="R18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S18" t="s">
         <v>45</v>
       </c>
       <c r="T18" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="U18" s="1">
-        <v>13618767.0300002</v>
+        <v>797851921.26</v>
       </c>
     </row>
     <row r="19">
@@ -926,29 +932,29 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
+      <c r="J19" t="s">
         <v>53</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
       <c r="K19" t="s">
         <v>37</v>
       </c>
@@ -971,16 +977,16 @@
         <v>43</v>
       </c>
       <c r="R19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="S19" t="s">
         <v>45</v>
       </c>
       <c r="T19" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="U19" s="1">
-        <v>224454884.07</v>
+        <v>1015306729.41</v>
       </c>
     </row>
     <row r="20">
@@ -991,29 +997,29 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
         <v>52</v>
       </c>
-      <c r="D20" t="s">
+      <c r="J20" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J20" t="s">
-        <v>58</v>
-      </c>
       <c r="K20" t="s">
         <v>37</v>
       </c>
@@ -1036,16 +1042,16 @@
         <v>43</v>
       </c>
       <c r="R20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S20" t="s">
         <v>45</v>
       </c>
       <c r="T20" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="U20" s="1">
-        <v>0</v>
+        <v>734100457.94</v>
       </c>
     </row>
     <row r="21">
@@ -1056,28 +1062,28 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s">
         <v>37</v>
@@ -1101,16 +1107,16 @@
         <v>43</v>
       </c>
       <c r="R21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S21" t="s">
         <v>45</v>
       </c>
       <c r="T21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="U21" s="1">
-        <v>0</v>
+        <v>224454884.07</v>
       </c>
     </row>
     <row r="22">
@@ -1121,28 +1127,28 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K22" t="s">
         <v>37</v>
@@ -1166,13 +1172,13 @@
         <v>43</v>
       </c>
       <c r="R22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S22" t="s">
         <v>45</v>
       </c>
       <c r="T22" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="U22" s="1">
         <v>0</v>
@@ -1186,22 +1192,22 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I23" t="s">
         <v>59</v>
@@ -1231,16 +1237,16 @@
         <v>43</v>
       </c>
       <c r="R23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S23" t="s">
         <v>45</v>
       </c>
       <c r="T23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="U23" s="1">
-        <v>30335525246.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1251,22 +1257,22 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I24" t="s">
         <v>59</v>
@@ -1296,16 +1302,16 @@
         <v>43</v>
       </c>
       <c r="R24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="S24" t="s">
         <v>45</v>
       </c>
       <c r="T24" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="U24" s="1">
-        <v>245.199996948242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1316,22 +1322,22 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I25" t="s">
         <v>59</v>
@@ -1361,16 +1367,16 @@
         <v>43</v>
       </c>
       <c r="R25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="S25" t="s">
         <v>45</v>
       </c>
       <c r="T25" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="U25" s="1">
-        <v>48.5999984741211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1381,28 +1387,28 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K26" t="s">
         <v>37</v>
@@ -1426,16 +1432,16 @@
         <v>43</v>
       </c>
       <c r="R26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S26" t="s">
         <v>45</v>
       </c>
       <c r="T26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="U26" s="1">
-        <v>0</v>
+        <v>30335525246.37</v>
       </c>
     </row>
     <row r="27">
@@ -1446,22 +1452,22 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I27" t="s">
         <v>61</v>
@@ -1491,16 +1497,16 @@
         <v>43</v>
       </c>
       <c r="R27" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S27" t="s">
         <v>45</v>
       </c>
       <c r="T27" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="U27" s="1">
-        <v>4836901875.42</v>
+        <v>245.199996948242</v>
       </c>
     </row>
     <row r="28">
@@ -1511,22 +1517,22 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I28" t="s">
         <v>61</v>
@@ -1556,16 +1562,16 @@
         <v>43</v>
       </c>
       <c r="R28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S28" t="s">
         <v>45</v>
       </c>
       <c r="T28" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="U28" s="1">
-        <v>0</v>
+        <v>48.5999984741211</v>
       </c>
     </row>
     <row r="29">
@@ -1576,22 +1582,22 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I29" t="s">
         <v>61</v>
@@ -1621,13 +1627,13 @@
         <v>43</v>
       </c>
       <c r="R29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S29" t="s">
         <v>45</v>
       </c>
       <c r="T29" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="U29" s="1">
         <v>0</v>
@@ -1641,22 +1647,22 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I30" t="s">
         <v>61</v>
@@ -1686,16 +1692,16 @@
         <v>43</v>
       </c>
       <c r="R30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S30" t="s">
         <v>45</v>
       </c>
       <c r="T30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U30" s="1">
-        <v>0</v>
+        <v>733.600002288818</v>
       </c>
     </row>
     <row r="31">
@@ -1706,29 +1712,29 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" t="s">
         <v>63</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>64</v>
       </c>
-      <c r="I31" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" t="s">
-        <v>58</v>
-      </c>
       <c r="K31" t="s">
         <v>37</v>
       </c>
@@ -1751,16 +1757,16 @@
         <v>43</v>
       </c>
       <c r="R31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S31" t="s">
         <v>45</v>
       </c>
       <c r="T31" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="U31" s="1">
-        <v>222640083.59</v>
+        <v>4836901875.42</v>
       </c>
     </row>
     <row r="32">
@@ -1771,29 +1777,29 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" t="s">
         <v>63</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>64</v>
       </c>
-      <c r="I32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" t="s">
-        <v>58</v>
-      </c>
       <c r="K32" t="s">
         <v>37</v>
       </c>
@@ -1816,16 +1822,16 @@
         <v>43</v>
       </c>
       <c r="R32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S32" t="s">
         <v>45</v>
       </c>
       <c r="T32" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U32" s="1">
-        <v>230639690.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1836,29 +1842,29 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" t="s">
         <v>63</v>
       </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>64</v>
       </c>
-      <c r="I33" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" t="s">
-        <v>58</v>
-      </c>
       <c r="K33" t="s">
         <v>37</v>
       </c>
@@ -1881,13 +1887,13 @@
         <v>43</v>
       </c>
       <c r="R33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S33" t="s">
         <v>45</v>
       </c>
       <c r="T33" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="U33" s="1">
         <v>0</v>
@@ -1901,29 +1907,29 @@
         <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" t="s">
         <v>63</v>
       </c>
-      <c r="H34" t="s">
+      <c r="J34" t="s">
         <v>64</v>
       </c>
-      <c r="I34" t="s">
-        <v>59</v>
-      </c>
-      <c r="J34" t="s">
-        <v>60</v>
-      </c>
       <c r="K34" t="s">
         <v>37</v>
       </c>
@@ -1946,16 +1952,16 @@
         <v>43</v>
       </c>
       <c r="R34" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="S34" t="s">
         <v>45</v>
       </c>
       <c r="T34" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="U34" s="1">
-        <v>7215805878.06</v>
+        <v>1756034.59999943</v>
       </c>
     </row>
     <row r="35">
@@ -1966,29 +1972,29 @@
         <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" t="s">
         <v>63</v>
       </c>
-      <c r="H35" t="s">
+      <c r="J35" t="s">
         <v>64</v>
       </c>
-      <c r="I35" t="s">
-        <v>59</v>
-      </c>
-      <c r="J35" t="s">
-        <v>60</v>
-      </c>
       <c r="K35" t="s">
         <v>37</v>
       </c>
@@ -2011,16 +2017,16 @@
         <v>43</v>
       </c>
       <c r="R35" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S35" t="s">
         <v>45</v>
       </c>
       <c r="T35" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="U35" s="1">
-        <v>39754702377.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2031,22 +2037,22 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I36" t="s">
         <v>59</v>
@@ -2076,16 +2082,16 @@
         <v>43</v>
       </c>
       <c r="R36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S36" t="s">
         <v>45</v>
       </c>
       <c r="T36" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="U36" s="1">
-        <v>39217018162.01</v>
+        <v>222640083.59</v>
       </c>
     </row>
     <row r="37">
@@ -2096,22 +2102,22 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G37" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I37" t="s">
         <v>59</v>
@@ -2141,16 +2147,16 @@
         <v>43</v>
       </c>
       <c r="R37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S37" t="s">
         <v>45</v>
       </c>
       <c r="T37" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="U37" s="1">
-        <v>33750147148.66</v>
+        <v>230639690.43</v>
       </c>
     </row>
     <row r="38">
@@ -2161,28 +2167,28 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G38" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H38" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K38" t="s">
         <v>37</v>
@@ -2206,16 +2212,16 @@
         <v>43</v>
       </c>
       <c r="R38" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="S38" t="s">
         <v>45</v>
       </c>
       <c r="T38" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="U38" s="1">
-        <v>5063324510.83</v>
+        <v>220619258.17</v>
       </c>
     </row>
     <row r="39">
@@ -2226,28 +2232,28 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F39" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H39" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K39" t="s">
         <v>37</v>
@@ -2271,16 +2277,16 @@
         <v>43</v>
       </c>
       <c r="R39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="S39" t="s">
         <v>45</v>
       </c>
       <c r="T39" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="U39" s="1">
-        <v>10321609207.42</v>
+        <v>235610924.47</v>
       </c>
     </row>
     <row r="40">
@@ -2291,22 +2297,22 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G40" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I40" t="s">
         <v>61</v>
@@ -2336,16 +2342,16 @@
         <v>43</v>
       </c>
       <c r="R40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S40" t="s">
         <v>45</v>
       </c>
       <c r="T40" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="U40" s="1">
-        <v>10256563585.45</v>
+        <v>7215805878.06</v>
       </c>
     </row>
     <row r="41">
@@ -2356,22 +2362,22 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G41" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H41" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I41" t="s">
         <v>61</v>
@@ -2401,16 +2407,536 @@
         <v>43</v>
       </c>
       <c r="R41" t="s">
+        <v>46</v>
+      </c>
+      <c r="S41" t="s">
+        <v>45</v>
+      </c>
+      <c r="T41" t="s">
+        <v>27</v>
+      </c>
+      <c r="U41" s="1">
+        <v>39754702377.41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" t="s">
+        <v>41</v>
+      </c>
+      <c r="P42" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>43</v>
+      </c>
+      <c r="R42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S42" t="s">
+        <v>45</v>
+      </c>
+      <c r="T42" t="s">
+        <v>37</v>
+      </c>
+      <c r="U42" s="1">
+        <v>39217018162.01</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" t="s">
+        <v>61</v>
+      </c>
+      <c r="J43" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" t="s">
+        <v>38</v>
+      </c>
+      <c r="M43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N43" t="s">
+        <v>40</v>
+      </c>
+      <c r="O43" t="s">
+        <v>41</v>
+      </c>
+      <c r="P43" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>43</v>
+      </c>
+      <c r="R43" t="s">
         <v>48</v>
       </c>
-      <c r="S41" t="s">
-        <v>45</v>
-      </c>
-      <c r="T41" t="s">
+      <c r="S43" t="s">
+        <v>45</v>
+      </c>
+      <c r="T43" t="s">
         <v>49</v>
       </c>
-      <c r="U41" s="1">
-        <v>5210512888.76</v>
+      <c r="U43" s="1">
+        <v>41970977264.11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" t="s">
+        <v>61</v>
+      </c>
+      <c r="J44" t="s">
+        <v>62</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M44" t="s">
+        <v>39</v>
+      </c>
+      <c r="N44" t="s">
+        <v>40</v>
+      </c>
+      <c r="O44" t="s">
+        <v>41</v>
+      </c>
+      <c r="P44" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>43</v>
+      </c>
+      <c r="R44" t="s">
+        <v>50</v>
+      </c>
+      <c r="S44" t="s">
+        <v>45</v>
+      </c>
+      <c r="T44" t="s">
+        <v>51</v>
+      </c>
+      <c r="U44" s="1">
+        <v>60235127217.76</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" t="s">
+        <v>65</v>
+      </c>
+      <c r="H45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I45" t="s">
+        <v>63</v>
+      </c>
+      <c r="J45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" t="s">
+        <v>38</v>
+      </c>
+      <c r="M45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O45" t="s">
+        <v>41</v>
+      </c>
+      <c r="P45" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>43</v>
+      </c>
+      <c r="R45" t="s">
+        <v>44</v>
+      </c>
+      <c r="S45" t="s">
+        <v>45</v>
+      </c>
+      <c r="T45" t="s">
+        <v>41</v>
+      </c>
+      <c r="U45" s="1">
+        <v>5063324510.83</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46" t="s">
+        <v>66</v>
+      </c>
+      <c r="I46" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" t="s">
+        <v>38</v>
+      </c>
+      <c r="M46" t="s">
+        <v>39</v>
+      </c>
+      <c r="N46" t="s">
+        <v>40</v>
+      </c>
+      <c r="O46" t="s">
+        <v>41</v>
+      </c>
+      <c r="P46" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" t="s">
+        <v>46</v>
+      </c>
+      <c r="S46" t="s">
+        <v>45</v>
+      </c>
+      <c r="T46" t="s">
+        <v>27</v>
+      </c>
+      <c r="U46" s="1">
+        <v>10321609207.42</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" t="s">
+        <v>66</v>
+      </c>
+      <c r="I47" t="s">
+        <v>63</v>
+      </c>
+      <c r="J47" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="L47" t="s">
+        <v>38</v>
+      </c>
+      <c r="M47" t="s">
+        <v>39</v>
+      </c>
+      <c r="N47" t="s">
+        <v>40</v>
+      </c>
+      <c r="O47" t="s">
+        <v>41</v>
+      </c>
+      <c r="P47" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" t="s">
+        <v>47</v>
+      </c>
+      <c r="S47" t="s">
+        <v>45</v>
+      </c>
+      <c r="T47" t="s">
+        <v>37</v>
+      </c>
+      <c r="U47" s="1">
+        <v>10256563585.45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I48" t="s">
+        <v>63</v>
+      </c>
+      <c r="J48" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L48" t="s">
+        <v>38</v>
+      </c>
+      <c r="M48" t="s">
+        <v>39</v>
+      </c>
+      <c r="N48" t="s">
+        <v>40</v>
+      </c>
+      <c r="O48" t="s">
+        <v>41</v>
+      </c>
+      <c r="P48" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>43</v>
+      </c>
+      <c r="R48" t="s">
+        <v>48</v>
+      </c>
+      <c r="S48" t="s">
+        <v>45</v>
+      </c>
+      <c r="T48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U48" s="1">
+        <v>12968115316.69</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" t="s">
+        <v>65</v>
+      </c>
+      <c r="H49" t="s">
+        <v>66</v>
+      </c>
+      <c r="I49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J49" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" t="s">
+        <v>38</v>
+      </c>
+      <c r="M49" t="s">
+        <v>39</v>
+      </c>
+      <c r="N49" t="s">
+        <v>40</v>
+      </c>
+      <c r="O49" t="s">
+        <v>41</v>
+      </c>
+      <c r="P49" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>43</v>
+      </c>
+      <c r="R49" t="s">
+        <v>50</v>
+      </c>
+      <c r="S49" t="s">
+        <v>45</v>
+      </c>
+      <c r="T49" t="s">
+        <v>51</v>
+      </c>
+      <c r="U49" s="1">
+        <v>13358543596.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>